<commit_message>
Sprint Plan 4 and updated burndown
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uk8535\Desktop\USM\5 Spring 2018\424\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabe\source\repos\Down2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,8 +78,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -91,7 +120,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -138,7 +167,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -202,20 +230,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$9</c:f>
@@ -223,25 +237,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -253,15 +267,29 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>136</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
+                <c:pt idx="1">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6642-4FBE-A2D4-AB0C3C71AC7C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -321,7 +349,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -439,7 +466,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1128,7 +1154,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1412,7 +1444,7 @@
   <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,49 +1465,83 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>136</v>
+        <v>221</v>
       </c>
       <c r="C3">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>82</v>
+        <f>(B3 - C3)</f>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>D3</f>
+        <v>201</v>
+      </c>
+      <c r="C4">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <f>(B4 - C4)</f>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <f>D4</f>
+        <v>165</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <f>(B5 - C5)</f>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <f>D5</f>
+        <v>144</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <f>(B6 - C6)</f>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DBConnect class and Sprint 4 presentation
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -200,7 +200,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -209,8 +209,10 @@
             <c:v>Trajectory</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -237,25 +239,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -281,13 +283,80 @@
                 <c:pt idx="4">
                   <c:v>84</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6642-4FBE-A2D4-AB0C3C71AC7C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-DB02-40F6-95BE-3C3536E54834}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1149,7 +1218,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1441,15 +1510,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A2:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1462,10 +1531,16 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>221</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>221</v>
@@ -1477,10 +1552,16 @@
         <f>(B3 - C3)</f>
         <v>201</v>
       </c>
+      <c r="O3">
+        <v>7</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <f>D3</f>
@@ -1494,9 +1575,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <f>D4</f>
@@ -1510,9 +1591,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <f>D5</f>
@@ -1526,22 +1607,25 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>